<commit_message>
Updated water depth data with variable flows
</commit_message>
<xml_diff>
--- a/Data/Water_Depth_From_Discharge.xlsx
+++ b/Data/Water_Depth_From_Discharge.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/LinaBarbosa/Documents/GitHub/Model/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elise\Desktop\GitHub\sparrow925.github.io\Model\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="640" yWindow="1180" windowWidth="24960" windowHeight="13500" tabRatio="500"/>
+    <workbookView xWindow="645" yWindow="1185" windowWidth="24960" windowHeight="13500" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="varslopes" sheetId="2" r:id="rId1"/>
+    <sheet name="Hoja1" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
   <si>
     <t>Section</t>
   </si>
@@ -41,11 +42,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="175" formatCode="0.00000000000"/>
+    <numFmt numFmtId="164" formatCode="0.00000000000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -81,7 +82,7 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -94,14 +95,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-CO"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -119,10 +123,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.132797498673322"/>
-          <c:y val="0.0329113924050633"/>
-          <c:w val="0.807093211709192"/>
-          <c:h val="0.8514135353334"/>
+          <c:x val="0.10676381570221027"/>
+          <c:y val="3.29113924050633E-2"/>
+          <c:w val="0.83312693685111716"/>
+          <c:h val="0.85141353533340003"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -148,143 +152,148 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Hoja1!$A$2:$A$21</c:f>
+              <c:f>varslopes!$A$2:$A$21</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7.0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>11.0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>12.0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>13.0</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>14.0</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>15.0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>16.0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>17.0</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>18.0</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>19.0</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hoja1!$B$2:$B$21</c:f>
+              <c:f>varslopes!$B$2:$B$21</c:f>
               <c:numCache>
-                <c:formatCode>0.00000000000</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>0.227399999999991</c:v>
+                  <c:v>0.25779999999998798</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.181999999999996</c:v>
+                  <c:v>0.20889999999999301</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.308399999999982</c:v>
+                  <c:v>0.32339999999998098</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.257099999999988</c:v>
+                  <c:v>0.23149999999999099</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.254099999999988</c:v>
+                  <c:v>0.245499999999989</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.281499999999985</c:v>
+                  <c:v>0.37339999999997497</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.164499999999998</c:v>
+                  <c:v>0.15459999999999899</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.193299999999995</c:v>
+                  <c:v>0.23329999999999099</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.232599999999991</c:v>
+                  <c:v>0.31509999999998201</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.276099999999986</c:v>
+                  <c:v>0.46289999999996501</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.568199999999954</c:v>
+                  <c:v>0.93269999999991404</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.32709999999998</c:v>
+                  <c:v>0.45279999999996601</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.438399999999968</c:v>
+                  <c:v>0.57519999999995297</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.384899999999974</c:v>
+                  <c:v>0.397399999999973</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.380499999999974</c:v>
+                  <c:v>0.31149999999998201</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.270299999999987</c:v>
+                  <c:v>0.23989999999999001</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.259899999999988</c:v>
+                  <c:v>0.22719999999999099</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.169799999999998</c:v>
+                  <c:v>0.141400000000001</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.350399999999978</c:v>
+                  <c:v>0.30769999999998199</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.127400000000002</c:v>
+                  <c:v>0.119900000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B172-4C72-AA79-7ACFB356FC80}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -306,143 +315,148 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Hoja1!$A$2:$A$21</c:f>
+              <c:f>varslopes!$A$2:$A$21</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7.0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>11.0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>12.0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>13.0</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>14.0</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>15.0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>16.0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>17.0</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>18.0</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>19.0</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hoja1!$C$2:$C$21</c:f>
+              <c:f>varslopes!$C$2:$C$21</c:f>
               <c:numCache>
-                <c:formatCode>0.00000000000</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>0.209999999999993</c:v>
+                  <c:v>0.23819999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.167399999999998</c:v>
+                  <c:v>0.19219999999999501</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.283999999999985</c:v>
+                  <c:v>0.29779999999998402</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.23639999999999</c:v>
+                  <c:v>0.21269999999999301</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.233599999999991</c:v>
+                  <c:v>0.225599999999991</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.259199999999988</c:v>
+                  <c:v>0.343899999999978</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.1514</c:v>
+                  <c:v>0.14220000000000099</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.177399999999997</c:v>
+                  <c:v>0.213999999999993</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.213599999999993</c:v>
+                  <c:v>0.28919999999998403</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.254099999999988</c:v>
+                  <c:v>0.42649999999996902</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.520499999999959</c:v>
+                  <c:v>0.85769999999992197</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.305199999999983</c:v>
+                  <c:v>0.42359999999997</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.404599999999972</c:v>
+                  <c:v>0.53169999999995798</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.356799999999977</c:v>
+                  <c:v>0.36839999999997602</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.353799999999977</c:v>
+                  <c:v>0.28899999999998399</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.249099999999989</c:v>
+                  <c:v>0.22099999999999201</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.24029999999999</c:v>
+                  <c:v>0.20979999999999299</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.156199999999999</c:v>
+                  <c:v>0.130000000000002</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.324799999999981</c:v>
+                  <c:v>0.28479999999998501</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.117000000000002</c:v>
+                  <c:v>0.110200000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-B172-4C72-AA79-7ACFB356FC80}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -464,143 +478,148 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Hoja1!$A$2:$A$21</c:f>
+              <c:f>varslopes!$A$2:$A$21</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7.0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>11.0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>12.0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>13.0</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>14.0</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>15.0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>16.0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>17.0</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>18.0</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>19.0</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hoja1!$D$2:$D$21</c:f>
+              <c:f>varslopes!$D$2:$D$21</c:f>
               <c:numCache>
-                <c:formatCode>0.00000000000</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>0.069400000000001</c:v>
+                  <c:v>7.9400000000001206E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0538000000000005</c:v>
+                  <c:v>6.20000000000007E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0910000000000016</c:v>
+                  <c:v>9.5800000000001703E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0752000000000011</c:v>
+                  <c:v>6.7900000000000904E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0742000000000011</c:v>
+                  <c:v>7.1900000000001005E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.0832000000000014</c:v>
+                  <c:v>0.111400000000002</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.0486000000000004</c:v>
+                  <c:v>4.5800000000000299E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.0559000000000006</c:v>
+                  <c:v>6.7500000000000906E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.0674000000000009</c:v>
+                  <c:v>9.1400000000001605E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.0813000000000013</c:v>
+                  <c:v>0.13820000000000099</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.154499999999999</c:v>
+                  <c:v>0.260699999999988</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.112200000000002</c:v>
+                  <c:v>0.16269999999999801</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.130300000000002</c:v>
+                  <c:v>0.174899999999997</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.121200000000002</c:v>
+                  <c:v>0.12590000000000201</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.123800000000003</c:v>
+                  <c:v>9.9600000000001798E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.0807000000000013</c:v>
+                  <c:v>7.1700000000000999E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.0800000000000013</c:v>
+                  <c:v>6.9600000000000994E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.0501000000000004</c:v>
+                  <c:v>4.1800000000000198E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.110300000000002</c:v>
+                  <c:v>9.6100000000001698E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.0372</c:v>
+                  <c:v>3.5200000000000002E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-B172-4C72-AA79-7ACFB356FC80}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -617,8 +636,8 @@
         <c:axId val="2124644688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="20.0"/>
-          <c:min val="1.0"/>
+          <c:max val="20"/>
+          <c:min val="1"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -678,8 +697,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.475565308434806"/>
-              <c:y val="0.938721419316256"/>
+              <c:x val="0.47556530843480599"/>
+              <c:y val="0.93872141931625597"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -707,7 +726,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-ES_tradnl"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -739,7 +758,899 @@
                 <a:cs typeface="Times New Roman" charset="0"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES_tradnl"/>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2136022640"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2136022640"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1100" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" charset="0"/>
+                    <a:ea typeface="Times New Roman" charset="0"/>
+                    <a:cs typeface="Times New Roman" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-ES_tradnl" sz="1100" b="1">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" charset="0"/>
+                    <a:ea typeface="Times New Roman" charset="0"/>
+                    <a:cs typeface="Times New Roman" charset="0"/>
+                  </a:rPr>
+                  <a:t>Water</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="es-ES_tradnl" sz="1100" b="1" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" charset="0"/>
+                    <a:ea typeface="Times New Roman" charset="0"/>
+                    <a:cs typeface="Times New Roman" charset="0"/>
+                  </a:rPr>
+                  <a:t> depth </a:t>
+                </a:r>
+                <a:br>
+                  <a:rPr lang="es-ES_tradnl" sz="1100" b="1" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" charset="0"/>
+                    <a:ea typeface="Times New Roman" charset="0"/>
+                    <a:cs typeface="Times New Roman" charset="0"/>
+                  </a:rPr>
+                </a:br>
+                <a:r>
+                  <a:rPr lang="es-ES_tradnl" sz="1100" b="1" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" charset="0"/>
+                    <a:ea typeface="Times New Roman" charset="0"/>
+                    <a:cs typeface="Times New Roman" charset="0"/>
+                  </a:rPr>
+                  <a:t>(meters)</a:t>
+                </a:r>
+                <a:endParaRPr lang="es-ES_tradnl" sz="1100" b="1">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:latin typeface="Times New Roman" charset="0"/>
+                  <a:ea typeface="Times New Roman" charset="0"/>
+                  <a:cs typeface="Times New Roman" charset="0"/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="1.8711700088024988E-2"/>
+              <c:y val="0.35020587049260354"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1100" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:latin typeface="Times New Roman" charset="0"/>
+                  <a:ea typeface="Times New Roman" charset="0"/>
+                  <a:cs typeface="Times New Roman" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" charset="0"/>
+                <a:ea typeface="Times New Roman" charset="0"/>
+                <a:cs typeface="Times New Roman" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2124644688"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.84608378870673895"/>
+          <c:y val="6.2536629123891102E-2"/>
+          <c:w val="0.103925390473732"/>
+          <c:h val="0.15234007774344699"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1100" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="Times New Roman" charset="0"/>
+              <a:ea typeface="Times New Roman" charset="0"/>
+              <a:cs typeface="Times New Roman" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.132797498673322"/>
+          <c:y val="3.29113924050633E-2"/>
+          <c:w val="0.80709321170919202"/>
+          <c:h val="0.85141353533340003"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Q460</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="002060"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Hoja1!$A$2:$A$21</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Hoja1!$B$2:$B$21</c:f>
+              <c:numCache>
+                <c:formatCode>0.00000000000</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>0.227399999999991</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.181999999999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.30839999999998202</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.257099999999988</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.254099999999988</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.28149999999998498</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.16449999999999801</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.193299999999995</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.23259999999999101</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.27609999999998602</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.56819999999995396</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.32709999999998002</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.43839999999996798</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.38489999999997399</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.38049999999997403</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.270299999999987</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.25989999999998797</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.16979999999999801</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.35039999999997801</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.12740000000000201</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-BA19-48BC-B63D-F2B42FD94EFF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Q400</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="0070C0"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Hoja1!$A$2:$A$21</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Hoja1!$C$2:$C$21</c:f>
+              <c:numCache>
+                <c:formatCode>0.00000000000</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>0.209999999999993</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.16739999999999799</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.28399999999998499</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.23639999999999001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.23359999999999101</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.259199999999988</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.15140000000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.177399999999997</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.21359999999999299</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.254099999999988</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.520499999999959</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.30519999999998298</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.40459999999997198</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.35679999999997702</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.35379999999997702</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.249099999999989</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.24029999999998999</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.15619999999999901</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.32479999999998099</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.11700000000000201</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-BA19-48BC-B63D-F2B42FD94EFF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Q60</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="00B0F0"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Hoja1!$A$2:$A$21</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Hoja1!$D$2:$D$21</c:f>
+              <c:numCache>
+                <c:formatCode>0.00000000000</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>6.9400000000001003E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.38000000000005E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.1000000000001594E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.5200000000001099E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.4200000000001098E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.3200000000001398E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.86000000000004E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.5900000000000602E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.7400000000000904E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8.1300000000001302E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.154499999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.11220000000000201</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.130300000000002</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.121200000000002</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.123800000000003</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8.0700000000001298E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8.0000000000001306E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5.0100000000000401E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.11030000000000199</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.7199999999999997E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-BA19-48BC-B63D-F2B42FD94EFF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2124644688"/>
+        <c:axId val="-2136022640"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2124644688"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="20"/>
+          <c:min val="1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-ES_tradnl" sz="1100" b="1">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" charset="0"/>
+                    <a:ea typeface="Times New Roman" charset="0"/>
+                    <a:cs typeface="Times New Roman" charset="0"/>
+                  </a:rPr>
+                  <a:t>Channel Polygon</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="es-ES_tradnl" sz="1100" b="1" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" charset="0"/>
+                    <a:ea typeface="Times New Roman" charset="0"/>
+                    <a:cs typeface="Times New Roman" charset="0"/>
+                  </a:rPr>
+                  <a:t> </a:t>
+                </a:r>
+                <a:endParaRPr lang="es-ES_tradnl" sz="1100" b="1">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:latin typeface="Times New Roman" charset="0"/>
+                  <a:ea typeface="Times New Roman" charset="0"/>
+                  <a:cs typeface="Times New Roman" charset="0"/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.47556530843480599"/>
+              <c:y val="0.93872141931625597"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" charset="0"/>
+                <a:ea typeface="Times New Roman" charset="0"/>
+                <a:cs typeface="Times New Roman" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="-2136022640"/>
@@ -829,8 +1740,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.0233059392166143"/>
-              <c:y val="0.325947174324728"/>
+              <c:x val="2.3305939216614301E-2"/>
+              <c:y val="0.32594717432472797"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -855,7 +1766,7 @@
                   <a:cs typeface="Times New Roman" charset="0"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-ES_tradnl"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -887,7 +1798,7 @@
                 <a:cs typeface="Times New Roman" charset="0"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES_tradnl"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2124644688"/>
@@ -908,10 +1819,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.846083788706739"/>
-          <c:y val="0.0625366291238911"/>
+          <c:x val="0.84608378870673895"/>
+          <c:y val="6.2536629123891102E-2"/>
           <c:w val="0.103925390473732"/>
-          <c:h val="0.152340077743447"/>
+          <c:h val="0.15234007774344699"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -936,7 +1847,7 @@
               <a:cs typeface="Times New Roman" charset="0"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-ES_tradnl"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -966,7 +1877,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-ES_tradnl"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1017,6 +1928,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1533,7 +2484,560 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>368300</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 4"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1833,18 +3337,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="23.83203125" customWidth="1"/>
-    <col min="3" max="3" width="20" customWidth="1"/>
-    <col min="4" max="4" width="18.83203125" customWidth="1"/>
+    <col min="1" max="1" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.77734375" customWidth="1"/>
+    <col min="3" max="3" width="17.109375" customWidth="1"/>
+    <col min="4" max="4" width="16.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1858,10 +3363,331 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" s="2">
         <v>1</v>
       </c>
+      <c r="B2">
+        <v>0.25779999999998798</v>
+      </c>
+      <c r="C2">
+        <v>0.23819999999999</v>
+      </c>
+      <c r="D2">
+        <v>7.9400000000001206E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>0.20889999999999301</v>
+      </c>
+      <c r="C3">
+        <v>0.19219999999999501</v>
+      </c>
+      <c r="D3">
+        <v>6.20000000000007E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>0.32339999999998098</v>
+      </c>
+      <c r="C4">
+        <v>0.29779999999998402</v>
+      </c>
+      <c r="D4">
+        <v>9.5800000000001703E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>0.23149999999999099</v>
+      </c>
+      <c r="C5">
+        <v>0.21269999999999301</v>
+      </c>
+      <c r="D5">
+        <v>6.7900000000000904E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>0.245499999999989</v>
+      </c>
+      <c r="C6">
+        <v>0.225599999999991</v>
+      </c>
+      <c r="D6">
+        <v>7.1900000000001005E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>0.37339999999997497</v>
+      </c>
+      <c r="C7">
+        <v>0.343899999999978</v>
+      </c>
+      <c r="D7">
+        <v>0.111400000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>0.15459999999999899</v>
+      </c>
+      <c r="C8">
+        <v>0.14220000000000099</v>
+      </c>
+      <c r="D8">
+        <v>4.5800000000000299E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>0.23329999999999099</v>
+      </c>
+      <c r="C9">
+        <v>0.213999999999993</v>
+      </c>
+      <c r="D9">
+        <v>6.7500000000000906E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>0.31509999999998201</v>
+      </c>
+      <c r="C10">
+        <v>0.28919999999998403</v>
+      </c>
+      <c r="D10">
+        <v>9.1400000000001605E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>0.46289999999996501</v>
+      </c>
+      <c r="C11">
+        <v>0.42649999999996902</v>
+      </c>
+      <c r="D11">
+        <v>0.13820000000000099</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>0.93269999999991404</v>
+      </c>
+      <c r="C12">
+        <v>0.85769999999992197</v>
+      </c>
+      <c r="D12">
+        <v>0.260699999999988</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="2">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>0.45279999999996601</v>
+      </c>
+      <c r="C13">
+        <v>0.42359999999997</v>
+      </c>
+      <c r="D13">
+        <v>0.16269999999999801</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="2">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>0.57519999999995297</v>
+      </c>
+      <c r="C14">
+        <v>0.53169999999995798</v>
+      </c>
+      <c r="D14">
+        <v>0.174899999999997</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="2">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>0.397399999999973</v>
+      </c>
+      <c r="C15">
+        <v>0.36839999999997602</v>
+      </c>
+      <c r="D15">
+        <v>0.12590000000000201</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="2">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>0.31149999999998201</v>
+      </c>
+      <c r="C16">
+        <v>0.28899999999998399</v>
+      </c>
+      <c r="D16">
+        <v>9.9600000000001798E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="2">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>0.23989999999999001</v>
+      </c>
+      <c r="C17">
+        <v>0.22099999999999201</v>
+      </c>
+      <c r="D17">
+        <v>7.1700000000000999E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="2">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>0.22719999999999099</v>
+      </c>
+      <c r="C18">
+        <v>0.20979999999999299</v>
+      </c>
+      <c r="D18">
+        <v>6.9600000000000994E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="2">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>0.141400000000001</v>
+      </c>
+      <c r="C19">
+        <v>0.130000000000002</v>
+      </c>
+      <c r="D19">
+        <v>4.1800000000000198E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="2">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>0.30769999999998199</v>
+      </c>
+      <c r="C20">
+        <v>0.28479999999998501</v>
+      </c>
+      <c r="D20">
+        <v>9.6100000000001698E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="2">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>0.119900000000002</v>
+      </c>
+      <c r="C21">
+        <v>0.110200000000002</v>
+      </c>
+      <c r="D21">
+        <v>3.5200000000000002E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D22"/>
+  <sheetViews>
+    <sheetView showRuler="0" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="A21" sqref="A1:A21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="23.77734375" customWidth="1"/>
+    <col min="3" max="3" width="20" customWidth="1"/>
+    <col min="4" max="4" width="18.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
       <c r="B2" s="3">
         <v>0.227399999999991</v>
       </c>
@@ -1872,7 +3698,7 @@
         <v>6.9400000000001003E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1886,7 +3712,7 @@
         <v>5.38000000000005E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1900,7 +3726,7 @@
         <v>9.1000000000001594E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1914,7 +3740,7 @@
         <v>7.5200000000001099E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1928,7 +3754,7 @@
         <v>7.4200000000001098E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1942,7 +3768,7 @@
         <v>8.3200000000001398E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1956,7 +3782,7 @@
         <v>4.86000000000004E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1970,7 +3796,7 @@
         <v>5.5900000000000602E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1984,7 +3810,7 @@
         <v>6.7400000000000904E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1998,7 +3824,7 @@
         <v>8.1300000000001302E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -2012,7 +3838,7 @@
         <v>0.154499999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -2026,7 +3852,7 @@
         <v>0.11220000000000201</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -2040,7 +3866,7 @@
         <v>0.130300000000002</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -2054,7 +3880,7 @@
         <v>0.121200000000002</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -2068,7 +3894,7 @@
         <v>0.123800000000003</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -2082,7 +3908,7 @@
         <v>8.0700000000001298E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -2096,7 +3922,7 @@
         <v>8.0000000000001306E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -2110,7 +3936,7 @@
         <v>5.0100000000000401E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -2124,7 +3950,7 @@
         <v>0.11030000000000199</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -2138,7 +3964,7 @@
         <v>3.7199999999999997E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>

</xml_diff>

<commit_message>
groundwork done for graph... but not quite good enough for presentation tomorrow.
</commit_message>
<xml_diff>
--- a/Data/Water_Depth_From_Discharge.xlsx
+++ b/Data/Water_Depth_From_Discharge.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="645" yWindow="1185" windowWidth="24960" windowHeight="13500" tabRatio="500"/>
+    <workbookView xWindow="645" yWindow="1185" windowWidth="24960" windowHeight="13500" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="varslopes" sheetId="2" r:id="rId1"/>
+    <sheet name="graphdata" sheetId="2" r:id="rId1"/>
     <sheet name="Hoja1" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150000"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
   <si>
     <t>Section</t>
   </si>
@@ -37,6 +37,12 @@
   </si>
   <si>
     <t>WaterDepth(Q60)</t>
+  </si>
+  <si>
+    <t>BankLow</t>
+  </si>
+  <si>
+    <t>Dist</t>
   </si>
 </sst>
 </file>
@@ -126,7 +132,7 @@
           <c:x val="0.10676381570221027"/>
           <c:y val="3.29113924050633E-2"/>
           <c:w val="0.83312693685111716"/>
-          <c:h val="0.85141353533340003"/>
+          <c:h val="0.84332724918819113"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -152,76 +158,76 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>varslopes!$A$2:$A$21</c:f>
+              <c:f>graphdata!$B$2:$B$21</c:f>
               <c:numCache>
-                <c:formatCode>0</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>4.0640000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>10.16</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>16.256</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>23.266400000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5</c:v>
+                  <c:v>29.362400000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6</c:v>
+                  <c:v>35.458399999999997</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7</c:v>
+                  <c:v>41.554400000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8</c:v>
+                  <c:v>47.650399999999998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9</c:v>
+                  <c:v>53.746400000000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10</c:v>
+                  <c:v>59.842399999999998</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>11</c:v>
+                  <c:v>65.938400000000001</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>12</c:v>
+                  <c:v>72.034400000000005</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>13</c:v>
+                  <c:v>87.2744</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>14</c:v>
+                  <c:v>102.51439999999999</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>15</c:v>
+                  <c:v>117.7544</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>16</c:v>
+                  <c:v>132.99440000000001</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>17</c:v>
+                  <c:v>148.23439999999999</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>18</c:v>
+                  <c:v>163.4744</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>19</c:v>
+                  <c:v>178.71440000000001</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>20</c:v>
+                  <c:v>187.85839999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>varslopes!$B$2:$B$21</c:f>
+              <c:f>graphdata!$D$2:$D$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -315,76 +321,76 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>varslopes!$A$2:$A$21</c:f>
+              <c:f>graphdata!$B$2:$B$21</c:f>
               <c:numCache>
-                <c:formatCode>0</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>4.0640000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>10.16</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>16.256</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>23.266400000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5</c:v>
+                  <c:v>29.362400000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6</c:v>
+                  <c:v>35.458399999999997</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7</c:v>
+                  <c:v>41.554400000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8</c:v>
+                  <c:v>47.650399999999998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9</c:v>
+                  <c:v>53.746400000000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10</c:v>
+                  <c:v>59.842399999999998</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>11</c:v>
+                  <c:v>65.938400000000001</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>12</c:v>
+                  <c:v>72.034400000000005</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>13</c:v>
+                  <c:v>87.2744</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>14</c:v>
+                  <c:v>102.51439999999999</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>15</c:v>
+                  <c:v>117.7544</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>16</c:v>
+                  <c:v>132.99440000000001</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>17</c:v>
+                  <c:v>148.23439999999999</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>18</c:v>
+                  <c:v>163.4744</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>19</c:v>
+                  <c:v>178.71440000000001</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>20</c:v>
+                  <c:v>187.85839999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>varslopes!$C$2:$C$21</c:f>
+              <c:f>graphdata!$E$2:$E$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -478,76 +484,76 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>varslopes!$A$2:$A$21</c:f>
+              <c:f>graphdata!$B$2:$B$21</c:f>
               <c:numCache>
-                <c:formatCode>0</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>4.0640000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>10.16</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>16.256</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>23.266400000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5</c:v>
+                  <c:v>29.362400000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6</c:v>
+                  <c:v>35.458399999999997</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7</c:v>
+                  <c:v>41.554400000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8</c:v>
+                  <c:v>47.650399999999998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9</c:v>
+                  <c:v>53.746400000000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10</c:v>
+                  <c:v>59.842399999999998</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>11</c:v>
+                  <c:v>65.938400000000001</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>12</c:v>
+                  <c:v>72.034400000000005</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>13</c:v>
+                  <c:v>87.2744</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>14</c:v>
+                  <c:v>102.51439999999999</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>15</c:v>
+                  <c:v>117.7544</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>16</c:v>
+                  <c:v>132.99440000000001</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>17</c:v>
+                  <c:v>148.23439999999999</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>18</c:v>
+                  <c:v>163.4744</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>19</c:v>
+                  <c:v>178.71440000000001</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>20</c:v>
+                  <c:v>187.85839999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>varslopes!$D$2:$D$21</c:f>
+              <c:f>graphdata!$F$2:$F$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -618,6 +624,172 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-B172-4C72-AA79-7ACFB356FC80}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Bank</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="50000"/>
+                  <a:alpha val="22000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>graphdata!$B$2:$B$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>4.0640000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16.256</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>23.266400000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>29.362400000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>35.458399999999997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>41.554400000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>47.650399999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>53.746400000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>59.842399999999998</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>65.938400000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>72.034400000000005</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>87.2744</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>102.51439999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>117.7544</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>132.99440000000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>148.23439999999999</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>163.4744</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>178.71440000000001</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>187.85839999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>graphdata!$C$2:$C$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.05</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.59</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.77</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.59</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.56000000000000005</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.85</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.56999999999999995</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D5C9-4F68-A599-D000D4F837D6}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -636,8 +808,8 @@
         <c:axId val="2124644688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="20"/>
-          <c:min val="1"/>
+          <c:max val="188"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -669,7 +841,28 @@
                     <a:ea typeface="Times New Roman" charset="0"/>
                     <a:cs typeface="Times New Roman" charset="0"/>
                   </a:rPr>
-                  <a:t>Channel Polygon</a:t>
+                  <a:t>Distance Along Channel</a:t>
+                </a:r>
+                <a:br>
+                  <a:rPr lang="es-ES_tradnl" sz="1100" b="1">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" charset="0"/>
+                    <a:ea typeface="Times New Roman" charset="0"/>
+                    <a:cs typeface="Times New Roman" charset="0"/>
+                  </a:rPr>
+                </a:br>
+                <a:r>
+                  <a:rPr lang="es-ES_tradnl" sz="1100" b="1">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" charset="0"/>
+                    <a:ea typeface="Times New Roman" charset="0"/>
+                    <a:cs typeface="Times New Roman" charset="0"/>
+                  </a:rPr>
+                  <a:t>(meters) </a:t>
                 </a:r>
                 <a:r>
                   <a:rPr lang="es-ES_tradnl" sz="1100" b="1" baseline="0">
@@ -730,7 +923,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -927,8 +1120,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.84608378870673895"/>
           <c:y val="6.2536629123891102E-2"/>
-          <c:w val="0.103925390473732"/>
-          <c:h val="0.15234007774344699"/>
+          <c:w val="8.4341561056782144E-2"/>
+          <c:h val="0.19469660632043637"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -3004,13 +3197,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>50800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>368300</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
@@ -3335,319 +3528,449 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="6.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.77734375" customWidth="1"/>
-    <col min="3" max="3" width="17.109375" customWidth="1"/>
-    <col min="4" max="4" width="16.5546875" customWidth="1"/>
+    <col min="2" max="3" width="6.88671875" customWidth="1"/>
+    <col min="4" max="4" width="16.77734375" customWidth="1"/>
+    <col min="5" max="5" width="17.109375" customWidth="1"/>
+    <col min="6" max="6" width="16.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="D1" s="1">
+        <v>460</v>
+      </c>
+      <c r="E1" s="1">
+        <v>400</v>
+      </c>
+      <c r="F1" s="1">
+        <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:6">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2">
+        <v>4.0640000000000001</v>
+      </c>
+      <c r="C2">
+        <f>0.5</f>
+        <v>0.5</v>
+      </c>
+      <c r="D2">
         <v>0.25779999999998798</v>
       </c>
-      <c r="C2">
+      <c r="E2">
         <v>0.23819999999999</v>
       </c>
-      <c r="D2">
+      <c r="F2">
         <v>7.9400000000001206E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:6">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3">
+        <v>10.16</v>
+      </c>
+      <c r="C3">
+        <v>0.45</v>
+      </c>
+      <c r="D3">
         <v>0.20889999999999301</v>
       </c>
-      <c r="C3">
+      <c r="E3">
         <v>0.19219999999999501</v>
       </c>
-      <c r="D3">
+      <c r="F3">
         <v>6.20000000000007E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:6">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4">
+        <v>16.256</v>
+      </c>
+      <c r="C4">
+        <v>0.75</v>
+      </c>
+      <c r="D4">
         <v>0.32339999999998098</v>
       </c>
-      <c r="C4">
+      <c r="E4">
         <v>0.29779999999998402</v>
       </c>
-      <c r="D4">
+      <c r="F4">
         <v>9.5800000000001703E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:6">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5">
+        <v>23.266400000000001</v>
+      </c>
+      <c r="C5">
+        <v>0.6</v>
+      </c>
+      <c r="D5">
         <v>0.23149999999999099</v>
       </c>
-      <c r="C5">
+      <c r="E5">
         <v>0.21269999999999301</v>
       </c>
-      <c r="D5">
+      <c r="F5">
         <v>6.7900000000000904E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:6">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6">
+        <v>29.362400000000001</v>
+      </c>
+      <c r="C6">
+        <v>0.35</v>
+      </c>
+      <c r="D6">
         <v>0.245499999999989</v>
       </c>
-      <c r="C6">
+      <c r="E6">
         <v>0.225599999999991</v>
       </c>
-      <c r="D6">
+      <c r="F6">
         <v>7.1900000000001005E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:6">
       <c r="A7" s="2">
         <v>6</v>
       </c>
       <c r="B7">
+        <v>35.458399999999997</v>
+      </c>
+      <c r="C7">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="D7">
         <v>0.37339999999997497</v>
       </c>
-      <c r="C7">
+      <c r="E7">
         <v>0.343899999999978</v>
       </c>
-      <c r="D7">
+      <c r="F7">
         <v>0.111400000000002</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:6">
       <c r="A8" s="2">
         <v>7</v>
       </c>
       <c r="B8">
+        <v>41.554400000000001</v>
+      </c>
+      <c r="C8">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="D8">
         <v>0.15459999999999899</v>
       </c>
-      <c r="C8">
+      <c r="E8">
         <v>0.14220000000000099</v>
       </c>
-      <c r="D8">
+      <c r="F8">
         <v>4.5800000000000299E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:6">
       <c r="A9" s="2">
         <v>8</v>
       </c>
       <c r="B9">
+        <v>47.650399999999998</v>
+      </c>
+      <c r="C9">
+        <v>0.7</v>
+      </c>
+      <c r="D9">
         <v>0.23329999999999099</v>
       </c>
-      <c r="C9">
+      <c r="E9">
         <v>0.213999999999993</v>
       </c>
-      <c r="D9">
+      <c r="F9">
         <v>6.7500000000000906E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:6">
       <c r="A10" s="2">
         <v>9</v>
       </c>
       <c r="B10">
+        <v>53.746400000000001</v>
+      </c>
+      <c r="C10">
+        <v>0.95</v>
+      </c>
+      <c r="D10">
         <v>0.31509999999998201</v>
       </c>
-      <c r="C10">
+      <c r="E10">
         <v>0.28919999999998403</v>
       </c>
-      <c r="D10">
+      <c r="F10">
         <v>9.1400000000001605E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:6">
       <c r="A11" s="2">
         <v>10</v>
       </c>
       <c r="B11">
+        <v>59.842399999999998</v>
+      </c>
+      <c r="C11">
+        <v>0.75</v>
+      </c>
+      <c r="D11">
         <v>0.46289999999996501</v>
       </c>
-      <c r="C11">
+      <c r="E11">
         <v>0.42649999999996902</v>
       </c>
-      <c r="D11">
+      <c r="F11">
         <v>0.13820000000000099</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:6">
       <c r="A12" s="2">
         <v>11</v>
       </c>
       <c r="B12">
+        <v>65.938400000000001</v>
+      </c>
+      <c r="C12">
+        <v>1.05</v>
+      </c>
+      <c r="D12">
         <v>0.93269999999991404</v>
       </c>
-      <c r="C12">
+      <c r="E12">
         <v>0.85769999999992197</v>
       </c>
-      <c r="D12">
+      <c r="F12">
         <v>0.260699999999988</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:6">
       <c r="A13" s="2">
         <v>12</v>
       </c>
       <c r="B13">
+        <v>72.034400000000005</v>
+      </c>
+      <c r="C13">
+        <v>0.59</v>
+      </c>
+      <c r="D13">
         <v>0.45279999999996601</v>
       </c>
-      <c r="C13">
+      <c r="E13">
         <v>0.42359999999997</v>
       </c>
-      <c r="D13">
+      <c r="F13">
         <v>0.16269999999999801</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:6">
       <c r="A14" s="2">
         <v>13</v>
       </c>
       <c r="B14">
+        <v>87.2744</v>
+      </c>
+      <c r="C14">
+        <v>0.8</v>
+      </c>
+      <c r="D14">
         <v>0.57519999999995297</v>
       </c>
-      <c r="C14">
+      <c r="E14">
         <v>0.53169999999995798</v>
       </c>
-      <c r="D14">
+      <c r="F14">
         <v>0.174899999999997</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:6">
       <c r="A15" s="2">
         <v>14</v>
       </c>
       <c r="B15">
+        <v>102.51439999999999</v>
+      </c>
+      <c r="C15">
+        <v>0.77</v>
+      </c>
+      <c r="D15">
         <v>0.397399999999973</v>
       </c>
-      <c r="C15">
+      <c r="E15">
         <v>0.36839999999997602</v>
       </c>
-      <c r="D15">
+      <c r="F15">
         <v>0.12590000000000201</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:6">
       <c r="A16" s="2">
         <v>15</v>
       </c>
       <c r="B16">
+        <v>117.7544</v>
+      </c>
+      <c r="C16">
+        <v>0.5</v>
+      </c>
+      <c r="D16">
         <v>0.31149999999998201</v>
       </c>
-      <c r="C16">
+      <c r="E16">
         <v>0.28899999999998399</v>
       </c>
-      <c r="D16">
+      <c r="F16">
         <v>9.9600000000001798E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:6">
       <c r="A17" s="2">
         <v>16</v>
       </c>
       <c r="B17">
+        <v>132.99440000000001</v>
+      </c>
+      <c r="C17">
+        <v>0.59</v>
+      </c>
+      <c r="D17">
         <v>0.23989999999999001</v>
       </c>
-      <c r="C17">
+      <c r="E17">
         <v>0.22099999999999201</v>
       </c>
-      <c r="D17">
+      <c r="F17">
         <v>7.1700000000000999E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:6">
       <c r="A18" s="2">
         <v>17</v>
       </c>
       <c r="B18">
+        <v>148.23439999999999</v>
+      </c>
+      <c r="C18">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="D18">
         <v>0.22719999999999099</v>
       </c>
-      <c r="C18">
+      <c r="E18">
         <v>0.20979999999999299</v>
       </c>
-      <c r="D18">
+      <c r="F18">
         <v>6.9600000000000994E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:6">
       <c r="A19" s="2">
         <v>18</v>
       </c>
       <c r="B19">
+        <v>163.4744</v>
+      </c>
+      <c r="C19">
+        <v>0.85</v>
+      </c>
+      <c r="D19">
         <v>0.141400000000001</v>
       </c>
-      <c r="C19">
+      <c r="E19">
         <v>0.130000000000002</v>
       </c>
-      <c r="D19">
+      <c r="F19">
         <v>4.1800000000000198E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:6">
       <c r="A20" s="2">
         <v>19</v>
       </c>
       <c r="B20">
+        <v>178.71440000000001</v>
+      </c>
+      <c r="C20">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="D20">
         <v>0.30769999999998199</v>
       </c>
-      <c r="C20">
+      <c r="E20">
         <v>0.28479999999998501</v>
       </c>
-      <c r="D20">
+      <c r="F20">
         <v>9.6100000000001698E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:6">
       <c r="A21" s="2">
         <v>20</v>
       </c>
       <c r="B21">
+        <v>187.85839999999999</v>
+      </c>
+      <c r="C21">
+        <v>0.8</v>
+      </c>
+      <c r="D21">
         <v>0.119900000000002</v>
       </c>
-      <c r="C21">
+      <c r="E21">
         <v>0.110200000000002</v>
       </c>
-      <c r="D21">
+      <c r="F21">
         <v>3.5200000000000002E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:6">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3659,7 +3982,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="D1" workbookViewId="0">
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="D1" workbookViewId="0">
       <selection activeCell="A21" sqref="A1:A21"/>
     </sheetView>
   </sheetViews>

</xml_diff>